<commit_message>
add namefile in seed2
</commit_message>
<xml_diff>
--- a/core/utils/distgradeunificadaUMUARAMA.xlsx
+++ b/core/utils/distgradeunificadaUMUARAMA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ventura System\Ventura Back-End\project-beck_ventura\core\utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SYS_EXPED_BACK\project-beck_ventura\core\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E8E85D-CA17-43A2-B13B-7EABE9542A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9336E1-806F-42CD-87E0-BDFD8CF05786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A7D8F346-A79E-4C25-BB45-DA9F96A70FA9}"/>
   </bookViews>
@@ -1007,9 +1007,9 @@
   <dimension ref="A1:U184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B157" sqref="B157"/>
+      <selection pane="bottomLeft" activeCell="S150" sqref="S150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6189,17 +6189,31 @@
         <v>42</v>
       </c>
       <c r="G148" s="11"/>
-      <c r="H148" s="11"/>
+      <c r="H148" s="11">
+        <v>8</v>
+      </c>
       <c r="I148" s="11"/>
       <c r="J148" s="11"/>
-      <c r="K148" s="11"/>
+      <c r="K148" s="11">
+        <v>8</v>
+      </c>
       <c r="L148" s="11"/>
-      <c r="M148" s="11"/>
-      <c r="N148" s="11"/>
-      <c r="O148" s="11"/>
-      <c r="P148" s="11"/>
+      <c r="M148" s="11">
+        <v>8</v>
+      </c>
+      <c r="N148" s="11">
+        <v>8</v>
+      </c>
+      <c r="O148" s="11">
+        <v>8</v>
+      </c>
+      <c r="P148" s="11">
+        <v>8</v>
+      </c>
       <c r="Q148" s="11"/>
-      <c r="R148" s="11"/>
+      <c r="R148" s="11">
+        <v>8</v>
+      </c>
       <c r="S148" s="11"/>
       <c r="T148" s="11"/>
       <c r="U148" s="11"/>

</xml_diff>